<commit_message>
pushing all my problems for posterity's sake
</commit_message>
<xml_diff>
--- a/extraction/lichen_nonusable_data.xlsx
+++ b/extraction/lichen_nonusable_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margaretslein/lichen/extraction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF74439-478B-FB46-98E2-2A0501FF01C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2469B2AC-1257-9F4F-9ABB-2D8B55B85252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16140" xr2:uid="{4ACB8208-C5EA-C743-ABBD-E40595E24DF5}"/>
   </bookViews>
@@ -613,13 +613,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3843665A-6476-F945-BA89-D583BCF376BB}">
   <dimension ref="A1:S349"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E88" workbookViewId="0">
-      <selection activeCell="N93" sqref="N93"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:O349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>

</xml_diff>